<commit_message>
Atualização do site e documentação
</commit_message>
<xml_diff>
--- a/documentacao/backlog.xlsx
+++ b/documentacao/backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cynth\OneDrive\Documentos\Cynthia\Faculdade\PI\Projeto individual\ProjetoIndividual\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CDBBF8-1832-4E02-B2C7-5A5BA5D925FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612DE1ED-8650-448D-A865-4C12763F5B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5DB1B81B-42BA-4FF4-9207-7E629BE541FE}"/>
   </bookViews>
@@ -184,7 +184,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,6 +227,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -266,12 +272,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -281,7 +281,15 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -290,8 +298,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFEFF789"/>
       <color rgb="FFF79F9F"/>
-      <color rgb="FFEFF789"/>
     </mruColors>
   </colors>
   <extLst>
@@ -622,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{165C460C-1183-4CFF-93AD-0113F1AA1A55}">
-  <dimension ref="B4:F25"/>
+  <dimension ref="B4:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -635,14 +643,14 @@
     <col min="4" max="4" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="2:4" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="B4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
@@ -653,125 +661,124 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="D6" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="D7" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="9"/>
-    </row>
-    <row r="10" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D11" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D12" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="D13" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D14" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D15" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -782,7 +789,7 @@
       <c r="C17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -793,7 +800,7 @@
       <c r="C18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -804,7 +811,7 @@
       <c r="C19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -815,8 +822,8 @@
       <c r="C20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>32</v>
+      <c r="D20" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -826,7 +833,7 @@
       <c r="C21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -837,7 +844,7 @@
       <c r="C22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -848,7 +855,7 @@
       <c r="C23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -859,7 +866,7 @@
       <c r="C24" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -870,7 +877,7 @@
       <c r="C25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="4" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
criação do conte sua historia
</commit_message>
<xml_diff>
--- a/documentacao/backlog.xlsx
+++ b/documentacao/backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cynth\OneDrive\Documentos\Cynthia\Faculdade\PI\Projeto individual\ProjetoIndividual\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612DE1ED-8650-448D-A865-4C12763F5B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24A34A3-60DE-4CA1-A7F2-E70641884496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5DB1B81B-42BA-4FF4-9207-7E629BE541FE}"/>
   </bookViews>
@@ -284,11 +284,11 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -632,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{165C460C-1183-4CFF-93AD-0113F1AA1A55}">
   <dimension ref="B4:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -644,11 +644,11 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:4" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
@@ -701,8 +701,8 @@
       <c r="C9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>31</v>
+      <c r="D9" s="6" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
@@ -712,8 +712,8 @@
       <c r="C10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>31</v>
+      <c r="D10" s="6" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
@@ -723,7 +723,7 @@
       <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="8" t="s">
         <v>32</v>
       </c>
     </row>
@@ -734,7 +734,7 @@
       <c r="C12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="8" t="s">
         <v>32</v>
       </c>
     </row>
@@ -745,7 +745,7 @@
       <c r="C13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="8" t="s">
         <v>32</v>
       </c>
     </row>
@@ -756,7 +756,7 @@
       <c r="C14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="8" t="s">
         <v>32</v>
       </c>
     </row>
@@ -767,7 +767,7 @@
       <c r="C15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="8" t="s">
         <v>32</v>
       </c>
     </row>
@@ -778,7 +778,7 @@
       <c r="C16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="8" t="s">
         <v>32</v>
       </c>
     </row>
@@ -789,7 +789,7 @@
       <c r="C17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="8" t="s">
         <v>32</v>
       </c>
     </row>
@@ -822,7 +822,7 @@
       <c r="C20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="8" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>